<commit_message>
end of Sep. 2018
</commit_message>
<xml_diff>
--- a/src/main/resources/Driving.xlsx
+++ b/src/main/resources/Driving.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4506"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B83028B3-7153-4487-A071-9CAEBF176399}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="12240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="12240"/>
   </bookViews>
   <sheets>
     <sheet name="Evcard" sheetId="1" r:id="rId1"/>
     <sheet name="Ponycar" sheetId="2" r:id="rId2"/>
     <sheet name="SUM" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179021"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -53,12 +52,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -66,13 +65,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -131,7 +130,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -401,24 +400,24 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1">
@@ -696,7 +695,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:3">
       <c r="A33" s="3">
         <v>43353</v>
       </c>
@@ -704,7 +703,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:3">
       <c r="A34" s="3">
         <v>43354</v>
       </c>
@@ -712,7 +711,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:3">
       <c r="A35" s="3">
         <v>43355</v>
       </c>
@@ -720,7 +719,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:3">
       <c r="A36" s="3">
         <v>43356</v>
       </c>
@@ -728,7 +727,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:3">
       <c r="A37" s="3">
         <v>43357</v>
       </c>
@@ -736,7 +735,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:3">
       <c r="A38" s="3">
         <v>43360</v>
       </c>
@@ -744,7 +743,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:3">
       <c r="A39" s="3">
         <v>43365</v>
       </c>
@@ -752,7 +751,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:3">
       <c r="A40" s="3">
         <v>43365</v>
       </c>
@@ -760,7 +759,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:3">
       <c r="A41" s="3">
         <v>43368</v>
       </c>
@@ -768,7 +767,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:3">
       <c r="A42" s="3">
         <v>43369</v>
       </c>
@@ -776,7 +775,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:3">
       <c r="A43" s="3">
         <v>43370</v>
       </c>
@@ -784,7 +783,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:3">
       <c r="A44" s="3">
         <v>43371</v>
       </c>
@@ -792,12 +791,16 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:3">
       <c r="A45" s="3">
         <v>43371</v>
       </c>
       <c r="B45" s="4">
         <v>5</v>
+      </c>
+      <c r="C45">
+        <f>SUM(B27:B45)</f>
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -808,17 +811,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1">
@@ -1096,7 +1099,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:3">
       <c r="A33" s="3">
         <v>43372</v>
       </c>
@@ -1104,12 +1107,32 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:3">
       <c r="A34" s="3">
         <v>43373</v>
       </c>
       <c r="B34" s="4">
         <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="3">
+        <v>43373</v>
+      </c>
+      <c r="B35" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="3">
+        <v>43373</v>
+      </c>
+      <c r="B36" s="4">
+        <v>14</v>
+      </c>
+      <c r="C36">
+        <f>SUM(B27:B36)</f>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1120,14 +1143,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
@@ -1144,7 +1167,7 @@
       </c>
       <c r="B3">
         <f>SUM(Ponycar!B:B)</f>
-        <v>303</v>
+        <v>321</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1161,7 +1184,7 @@
       </c>
       <c r="B5">
         <f>SUM(B2:B4)</f>
-        <v>1039.4000000000001</v>
+        <v>1057.4000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
at the end of 2018
</commit_message>
<xml_diff>
--- a/src/main/resources/Driving.xlsx
+++ b/src/main/resources/Driving.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B80316C8-035A-4E08-8C8F-8CDB1BE94C05}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B87C7090-9C1D-4CD3-B6C3-43BEDF19CA9A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="12240" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="12240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Evcard" sheetId="1" r:id="rId1"/>
@@ -432,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C88"/>
+  <dimension ref="A1:C89"/>
   <sheetViews>
     <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="B88" sqref="B88"/>
+      <selection activeCell="F80" sqref="F80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1179,6 +1179,18 @@
         <v>41</v>
       </c>
     </row>
+    <row r="89" spans="1:3">
+      <c r="A89" s="3">
+        <v>43465</v>
+      </c>
+      <c r="B89" s="4">
+        <v>3</v>
+      </c>
+      <c r="C89">
+        <f>SUM(B82:B89)</f>
+        <v>184</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1190,8 +1202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1615,7 +1627,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:3">
       <c r="A49" s="3">
         <v>43438</v>
       </c>
@@ -1623,7 +1635,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:3">
       <c r="A50" s="3">
         <v>43439</v>
       </c>
@@ -1631,12 +1643,16 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:3">
       <c r="A51" s="3">
         <v>43451</v>
       </c>
       <c r="B51" s="4">
         <v>12</v>
+      </c>
+      <c r="C51">
+        <f>SUM(B48:B51)</f>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1889,7 +1905,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A2:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
@@ -1901,7 +1917,7 @@
       </c>
       <c r="B2">
         <f>SUM(Evcard!B:B)</f>
-        <v>1169</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1955,7 +1971,7 @@
       </c>
       <c r="B8">
         <f>SUM(B2:B7)</f>
-        <v>2046.3</v>
+        <v>2049.3000000000002</v>
       </c>
     </row>
     <row r="11" spans="1:2">

</xml_diff>